<commit_message>
simple example to work out the code
</commit_message>
<xml_diff>
--- a/example_60187modified.xlsx
+++ b/example_60187modified.xlsx
@@ -207,7 +207,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -256,6 +256,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -271,7 +283,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -313,6 +325,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -917,8 +935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:C39"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
@@ -1123,7 +1141,7 @@
       <c r="C18" s="11"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
-      <c r="G18" s="10">
+      <c r="G18" s="14">
         <v>16.2</v>
       </c>
       <c r="H18" s="7" t="s">
@@ -1347,8 +1365,8 @@
       <c r="C39" s="12">
         <v>49.2</v>
       </c>
-      <c r="D39" s="7" t="s">
-        <v>21</v>
+      <c r="D39" s="15" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="40" spans="1:8">

</xml_diff>